<commit_message>
Signup save to userInforList
</commit_message>
<xml_diff>
--- a/designDocument/workman-description.xlsx
+++ b/designDocument/workman-description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{933DEBCA-68F5-4DDC-8007-0B6DEC926424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF33CE70-A64C-4C16-9BBA-276EBF677267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13820" yWindow="160" windowWidth="18680" windowHeight="9800" tabRatio="656" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
+    <workbookView xWindow="20640" yWindow="180" windowWidth="22830" windowHeight="14715" tabRatio="656" activeTab="1" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -979,7 +979,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>userInfor0 = [{ }, { }, { }, { }];</a:t>
+            <a:t>userInfor0 = [{ }, [ ], [ ],  [ ], [ ] ];</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1001,7 +1001,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>userInfor0 = [ user, itemsInCart, itemsInFavorite, itemsInSaved</a:t>
+            <a:t>userInfor0 = [ user, itemsInCart, itemsInFavorite, itemsInSaved, itemsBuyItAgain</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" baseline="0">
@@ -1050,8 +1050,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1210581" y="7210400"/>
-          <a:ext cx="7187293" cy="2834822"/>
+          <a:off x="1204382" y="7217960"/>
+          <a:ext cx="7256992" cy="2834822"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -1400,8 +1400,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1210581" y="1797958"/>
-          <a:ext cx="7187293" cy="2834822"/>
+          <a:off x="1204382" y="1805518"/>
+          <a:ext cx="7256992" cy="2834822"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -3604,8 +3604,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1210581" y="11751957"/>
-          <a:ext cx="7187293" cy="2831647"/>
+          <a:off x="1204382" y="11756342"/>
+          <a:ext cx="7256992" cy="2834822"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -6758,14 +6758,14 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>1682</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>145116</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>130970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>192181</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -6780,8 +6780,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10345832" y="4002741"/>
-          <a:ext cx="2686049" cy="1855133"/>
+          <a:off x="9621932" y="6655595"/>
+          <a:ext cx="2678905" cy="2059780"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6830,7 +6830,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6839,12 +6839,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>let userObject = {</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>function userObject(){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6853,12 +6853,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    userId: userId,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>    this.userId = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6867,10 +6867,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    fullName:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:t>    this.fullName = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6879,10 +6881,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> full</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>    this.userName = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6891,12 +6895,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Name,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>    this.email = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6905,12 +6909,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    userName: userName,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>    this.password = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6919,12 +6923,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    email: email,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>    type: "user";</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6933,10 +6937,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    password:</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
+            <a:t>    status: "normal"</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -6945,74 +6951,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> password</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>,</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    type: "user",</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    status: "normal" or "locked"</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
             <a:t>}</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -7023,7 +6963,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>120183</xdr:rowOff>
+      <xdr:rowOff>17860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
@@ -7046,8 +6986,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8734425" y="4930308"/>
-          <a:ext cx="1611407" cy="670392"/>
+          <a:off x="8017669" y="7685485"/>
+          <a:ext cx="1604263" cy="772715"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -8690,7 +8630,7 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0">
+            <a:rPr lang="en-US" sz="1400" b="0" strike="sngStrike" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -8699,12 +8639,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>let itemForOneUser = {</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+            <a:t>function itemForOneUser (){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" strike="sngStrike" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -8713,21 +8653,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    itemName: itemName,</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400" b="0">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+            <a:t>    this.itemId = [ ];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" strike="sngStrike" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -8736,12 +8667,12 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    itemId: [ ],</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
+            <a:t>    this.itemQuantity =[ ];</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" strike="sngStrike" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -8750,65 +8681,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>    itemQuantity: [ ],</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    itemPrice: [ ],</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    img: imgSource</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>    </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
             <a:t>}</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8819,13 +8693,13 @@
       <xdr:col>28</xdr:col>
       <xdr:colOff>4150</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>70694</xdr:rowOff>
+      <xdr:rowOff>144777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>549088</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>98418</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8840,8 +8714,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17811759" y="5644890"/>
-          <a:ext cx="2996590" cy="599224"/>
+          <a:off x="17138567" y="5722194"/>
+          <a:ext cx="3000271" cy="426723"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8885,12 +8759,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>//itemsInCart</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
+            <a:t>itemsInCart = [ ]; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -8899,33 +8771,17 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>let  itemsInCart =  new</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>itemForOneUser();</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+            <a:t>   //item Id only</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8935,14 +8791,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>4150</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>107235</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>11985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>134959</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8957,8 +8813,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17811759" y="6443431"/>
-          <a:ext cx="3019002" cy="599224"/>
+          <a:off x="17138567" y="7113402"/>
+          <a:ext cx="3022683" cy="474848"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8992,6 +8848,23 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1">
               <a:solidFill>
@@ -9002,46 +8875,24 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>//itemsInFavorite</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>let  itemsInFavorite =  new</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>itemForOneUser();</a:t>
-          </a:r>
+            <a:t>itemsInFavorite = [ ]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -9052,14 +8903,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>4150</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>179341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>582145</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>16565</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9074,8 +8925,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17811759" y="7277537"/>
-          <a:ext cx="3029647" cy="599224"/>
+          <a:off x="17138567" y="7852258"/>
+          <a:ext cx="3033328" cy="487410"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9109,6 +8960,23 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1">
               <a:solidFill>
@@ -9119,259 +8987,28 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>//itemsInSaved</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>let  itemsInSaved =  new</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>itemForOneUser();</a:t>
-          </a:r>
+            <a:t>itemsInSaved = [ ]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US">
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>389282</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100366</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>593911</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>100366</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="31" name="Straight Arrow Connector 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA38C259-6B49-4422-87DD-BE3109454A9F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="16358152" y="7579562"/>
-          <a:ext cx="1430455" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>484255</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>145745</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>484255</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>124239</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="47" name="Straight Connector 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{064CF3B1-225E-54EB-EB14-F29DC44B3DE5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17066038" y="5910441"/>
-          <a:ext cx="0" cy="1692994"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>459441</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>173448</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>582705</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>173448</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Straight Arrow Connector 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{946F4DA5-0B89-0041-1F07-8E5BCE37609E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17041224" y="5938144"/>
-          <a:ext cx="736177" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>488674</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>58953</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>582705</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>58953</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA1A219-7E79-AA36-63BC-8A571C3D6167}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17070457" y="6776149"/>
-          <a:ext cx="706944" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -10144,6 +9781,581 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>154781</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>314441</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>134269</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0947588C-3DB1-4E72-8C3C-5F8E3981852F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16513969" y="9882187"/>
+          <a:ext cx="1981316" cy="1920207"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>//Item object constructor</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>function item(){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.itemId = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.itemName = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.category = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.price = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.img = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.stock = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.type = 'item'</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>219191</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>134269</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="TextBox 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{665C0D6B-B4FA-40C4-975C-16E9F37A768E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18847594" y="9882187"/>
+          <a:ext cx="1981316" cy="1920207"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>//Item rating &amp; review object constructor</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>function itemRatingAndReview (){</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.itemId = '';</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.rating = 0;    //initial</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>    this.review = []</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>}</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>4150</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>134194</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>549088</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>179916</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="44" name="TextBox 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B358DAD2-F0B8-D4C6-7BB1-1FBEF57441E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17138567" y="8569111"/>
+          <a:ext cx="3000271" cy="426722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>itemsBuyItAgain = [ ]</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>179916</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>603250</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>179916</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Right Brace 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80A7A383-A99A-1E6E-5AB0-D43D1773267D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20002500" y="6900333"/>
+          <a:ext cx="804333" cy="2286000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>59530</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>55561</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>219190</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>10582</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="TextBox 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D59A1998-F55D-E259-AA88-A23C7C9C819B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="20876947" y="7728478"/>
+          <a:ext cx="2001160" cy="717021"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="2400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Optional</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="2400" b="0">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -21477,7 +21689,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A36A3AB-75F8-48A0-8E70-2629D6FB9237}">
   <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -21565,11 +21777,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D800F0-F99C-47B6-B0F4-3731F0185DB9}">
   <dimension ref="A1:AQ101"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="Q14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="R15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="U31" sqref="U31"/>
+      <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
SignUp and Login OK
</commit_message>
<xml_diff>
--- a/designDocument/workman-description.xlsx
+++ b/designDocument/workman-description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF33CE70-A64C-4C16-9BBA-276EBF677267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DCD1939-C62C-479B-89BB-B2EF8B95D379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="180" windowWidth="22830" windowHeight="14715" tabRatio="656" activeTab="1" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
+    <workbookView xWindow="14960" yWindow="480" windowWidth="18420" windowHeight="10130" tabRatio="656" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="97">
   <si>
     <t>customers</t>
   </si>
@@ -321,6 +321,9 @@
   <si>
     <t>Flag ở localStorage,  session</t>
   </si>
+  <si>
+    <t>*Thay alert bằng Snackbar</t>
+  </si>
 </sst>
 </file>
 
@@ -1050,8 +1053,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1204382" y="7217960"/>
-          <a:ext cx="7256992" cy="2834822"/>
+          <a:off x="1210581" y="7210400"/>
+          <a:ext cx="7187293" cy="2834822"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -1400,8 +1403,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1204382" y="1805518"/>
-          <a:ext cx="7256992" cy="2834822"/>
+          <a:off x="1210581" y="1797958"/>
+          <a:ext cx="7187293" cy="2834822"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -3604,8 +3607,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1204382" y="11756342"/>
-          <a:ext cx="7256992" cy="2834822"/>
+          <a:off x="1210581" y="11751957"/>
+          <a:ext cx="7187293" cy="2831647"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -21687,10 +21690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A36A3AB-75F8-48A0-8E70-2629D6FB9237}">
-  <dimension ref="B1:E11"/>
+  <dimension ref="B1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21767,6 +21770,11 @@
         <v>94</v>
       </c>
     </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -21777,11 +21785,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D800F0-F99C-47B6-B0F4-3731F0185DB9}">
   <dimension ref="A1:AQ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="R15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="X22" sqref="X22"/>
+      <selection pane="bottomRight" activeCell="AK31" sqref="AK31:AK32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
item edit Ok. fix small bug in snackbar and signup
</commit_message>
<xml_diff>
--- a/designDocument/workman-description.xlsx
+++ b/designDocument/workman-description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA623A7A-E366-4517-8ADE-50B3C41E62BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA7079F5-6BA0-4C07-B035-46CF5BB85E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2025" yWindow="435" windowWidth="17550" windowHeight="9720" tabRatio="709" activeTab="1" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="709" activeTab="8" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -343,7 +343,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -388,6 +388,12 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -416,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -459,7 +465,8 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -21928,7 +21935,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E11AF87-82A7-468A-8D96-81CF2BB39B7A}">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -21965,10 +21972,10 @@
   <dimension ref="A1:AQ101"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="M34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="F77" sqref="F77"/>
+      <selection pane="bottomRight" activeCell="Z85" sqref="Z85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23210,8 +23217,8 @@
   </sheetPr>
   <dimension ref="A2:F18"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23247,7 +23254,7 @@
       <c r="B3" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="18" t="s">
         <v>76</v>
       </c>
       <c r="D3" s="1">
@@ -23264,7 +23271,7 @@
       <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="1">
@@ -23281,7 +23288,7 @@
       <c r="B5" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="18" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="1">
@@ -23298,7 +23305,7 @@
       <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="1">
@@ -23315,7 +23322,7 @@
       <c r="B7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="18" t="s">
         <v>68</v>
       </c>
       <c r="D7" s="1">
@@ -23332,7 +23339,7 @@
       <c r="B8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="18" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="1">
@@ -23349,7 +23356,7 @@
       <c r="B9" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="19" t="s">
         <v>72</v>
       </c>
       <c r="D9" s="1">
@@ -23366,7 +23373,7 @@
       <c r="B10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D10" s="1">
@@ -23383,7 +23390,7 @@
       <c r="B11" t="s">
         <v>49</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="17" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="1">
@@ -23451,7 +23458,7 @@
       <c r="B15" t="s">
         <v>50</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="17" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="1">
@@ -23468,7 +23475,7 @@
       <c r="B16" t="s">
         <v>50</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="17" t="s">
         <v>63</v>
       </c>
       <c r="D16" s="1">
@@ -23514,5 +23521,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add to cart OK. 1user 1 cart OK.
</commit_message>
<xml_diff>
--- a/designDocument/workman-description.xlsx
+++ b/designDocument/workman-description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F2897F-8F51-457E-8CFD-50B41F26D5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59FEB3E-8B54-4619-9DBD-EFA1520609F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23115" yWindow="2460" windowWidth="17955" windowHeight="10965" tabRatio="709" activeTab="3" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
+    <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="709" activeTab="1" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
   <si>
     <t>customers</t>
   </si>
@@ -336,13 +336,25 @@
     <t>Admin</t>
   </si>
   <si>
-    <t>nút edit và lock chưa làm</t>
-  </si>
-  <si>
     <t>logo</t>
   </si>
   <si>
     <t>https://workman.jp/img/share/logo_workman_mark.svg</t>
+  </si>
+  <si>
+    <t>sessionStorage</t>
+  </si>
+  <si>
+    <t>whoIsLogIn</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>logInId</t>
+  </si>
+  <si>
+    <t>idOfUser</t>
   </si>
 </sst>
 </file>
@@ -952,7 +964,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>326200</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>88638</xdr:rowOff>
+      <xdr:rowOff>91813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1123,6 +1135,50 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>13093</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46937023-38B9-660A-3600-74C5ECB95982}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1657350" y="3048001"/>
+          <a:ext cx="4387850" cy="3442092"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1283,8 +1339,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1191931" y="7209867"/>
-          <a:ext cx="7161119" cy="2834822"/>
+          <a:off x="1198842" y="7340602"/>
+          <a:ext cx="7240120" cy="2890851"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -1633,8 +1689,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1198281" y="1797425"/>
-          <a:ext cx="7154769" cy="2834822"/>
+          <a:off x="1205192" y="1823572"/>
+          <a:ext cx="7233770" cy="2890851"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -3837,8 +3893,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1191931" y="11748249"/>
-          <a:ext cx="7161119" cy="2834822"/>
+          <a:off x="1198842" y="11971806"/>
+          <a:ext cx="7240120" cy="2887676"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -21834,7 +21890,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A36A3AB-75F8-48A0-8E70-2629D6FB9237}">
   <dimension ref="B1:E19"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -21939,10 +21995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E11AF87-82A7-468A-8D96-81CF2BB39B7A}">
-  <dimension ref="A2:C15"/>
+  <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21951,20 +22007,22 @@
     <col min="3" max="3" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
       </c>
-      <c r="C15" t="s">
-        <v>100</v>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -21978,10 +22036,10 @@
   <dimension ref="A1:AQ101"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="P34" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="X13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="P58" sqref="P58"/>
+      <selection pane="bottomRight" activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21989,6 +22047,7 @@
     <col min="1" max="1" width="7.42578125" customWidth="1"/>
     <col min="2" max="2" width="9.28515625" style="1" customWidth="1"/>
     <col min="20" max="20" width="10" customWidth="1"/>
+    <col min="24" max="24" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
@@ -22115,12 +22174,36 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="43:43" x14ac:dyDescent="0.25">
+    <row r="35" spans="24:43" x14ac:dyDescent="0.25">
       <c r="AQ35" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="64" spans="20:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="24:43" x14ac:dyDescent="0.25">
+      <c r="X47" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="48" spans="24:43" x14ac:dyDescent="0.25">
+      <c r="X48" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="20:25" x14ac:dyDescent="0.25">
+      <c r="X49" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="64" spans="20:25" x14ac:dyDescent="0.25">
       <c r="T64" s="9" t="s">
         <v>33</v>
       </c>
@@ -22391,7 +22474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55527AE-C7AB-4C6E-A279-E068211F1548}">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
@@ -22624,10 +22707,10 @@
     </row>
     <row r="60" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
+        <v>100</v>
+      </c>
+      <c r="F60" s="6" t="s">
         <v>101</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter by category. Sort by price OK
</commit_message>
<xml_diff>
--- a/designDocument/workman-description.xlsx
+++ b/designDocument/workman-description.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59FEB3E-8B54-4619-9DBD-EFA1520609F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D756F4-1297-4F57-91B4-03E9168A4C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13550" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="709" activeTab="1" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
+    <workbookView xWindow="1425" yWindow="795" windowWidth="15375" windowHeight="9210" tabRatio="709" activeTab="2" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
     <sheet name="baka" sheetId="9" r:id="rId2"/>
-    <sheet name="admin" sheetId="1" r:id="rId3"/>
-    <sheet name="shopping(index)" sheetId="4" r:id="rId4"/>
-    <sheet name="cart" sheetId="5" r:id="rId5"/>
-    <sheet name="sign up" sheetId="6" r:id="rId6"/>
-    <sheet name="login" sheetId="7" r:id="rId7"/>
-    <sheet name="function-desc" sheetId="2" r:id="rId8"/>
-    <sheet name="Item list" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId3"/>
+    <sheet name="admin" sheetId="1" r:id="rId4"/>
+    <sheet name="shopping(index)" sheetId="4" r:id="rId5"/>
+    <sheet name="cart" sheetId="5" r:id="rId6"/>
+    <sheet name="sign up" sheetId="6" r:id="rId7"/>
+    <sheet name="login" sheetId="7" r:id="rId8"/>
+    <sheet name="function-desc" sheetId="2" r:id="rId9"/>
+    <sheet name="Item list" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="108">
   <si>
     <t>customers</t>
   </si>
@@ -356,6 +357,9 @@
   <si>
     <t>idOfUser</t>
   </si>
+  <si>
+    <t>array sort</t>
+  </si>
 </sst>
 </file>
 
@@ -1144,9 +1148,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:colOff>320675</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>13093</xdr:rowOff>
+      <xdr:rowOff>16268</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1179,10 +1183,103 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>79230</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>278214</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>53619</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5943782-8A90-FFA4-CFEC-A88696D746CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1736580" y="6797675"/>
+          <a:ext cx="6098134" cy="1828444"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>522078</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>601639</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9020</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628DA9DE-41FC-FE6D-6270-B7900785D478}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="522078" y="549275"/>
+          <a:ext cx="8613961" cy="2698245"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -10562,7 +10659,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14637,7 +14734,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -15993,8 +16090,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3055284" y="3762856"/>
-          <a:ext cx="5412289" cy="2023225"/>
+          <a:off x="3050988" y="3837001"/>
+          <a:ext cx="5479524" cy="2057403"/>
           <a:chOff x="2085975" y="3793672"/>
           <a:chExt cx="5452630" cy="2023225"/>
         </a:xfrm>
@@ -19680,7 +19777,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -20854,7 +20951,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -21993,12 +22090,327 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D3853C-29D5-449B-8AA1-1129D3EE9DEA}">
+  <sheetPr>
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A2:F18"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1280</v>
+      </c>
+      <c r="E3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="1">
+        <v>580</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2780</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="1">
+        <v>980</v>
+      </c>
+      <c r="E6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="1">
+        <v>98</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1">
+        <v>190</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="1">
+        <v>290</v>
+      </c>
+      <c r="E9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1">
+        <v>150</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="1">
+        <v>98</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1">
+        <v>128</v>
+      </c>
+      <c r="E13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="1">
+        <v>190</v>
+      </c>
+      <c r="E14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1">
+        <v>49</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="1">
+        <v>98</v>
+      </c>
+      <c r="E16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="1">
+        <v>150</v>
+      </c>
+      <c r="E18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E11AF87-82A7-468A-8D96-81CF2BB39B7A}">
-  <dimension ref="A2:B17"/>
+  <dimension ref="A2:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22025,6 +22437,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -22032,6 +22452,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFD0586-BC3F-4075-B66A-03FF886CAA45}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D800F0-F99C-47B6-B0F4-3731F0185DB9}">
   <dimension ref="A1:AQ101"/>
   <sheetViews>
@@ -22470,7 +22905,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55527AE-C7AB-4C6E-A279-E068211F1548}">
   <dimension ref="A1:S60"/>
   <sheetViews>
@@ -22725,7 +23160,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726A8A91-2E1C-4E34-A304-FBDB9334D0CB}">
   <dimension ref="A1:V19"/>
   <sheetViews>
@@ -22897,7 +23332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B55669BA-C4BC-472D-A82C-F4DC422487C3}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -23066,7 +23501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EB38C6-79E9-4766-804E-372B2BE35E2E}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -23212,7 +23647,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1159BDC3-93C3-445C-9BEA-F7F6F82CBE48}">
   <dimension ref="B3:I10"/>
   <sheetViews>
@@ -23312,319 +23747,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D3853C-29D5-449B-8AA1-1129D3EE9DEA}">
-  <sheetPr>
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A2:F18"/>
-  <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" s="1">
-        <v>1280</v>
-      </c>
-      <c r="E3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="1">
-        <v>580</v>
-      </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="1">
-        <v>2780</v>
-      </c>
-      <c r="E5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="1">
-        <v>980</v>
-      </c>
-      <c r="E6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="1">
-        <v>98</v>
-      </c>
-      <c r="E7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="1">
-        <v>190</v>
-      </c>
-      <c r="E8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D9" s="1">
-        <v>290</v>
-      </c>
-      <c r="E9" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D10" s="1">
-        <v>150</v>
-      </c>
-      <c r="E10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="1">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="1">
-        <v>98</v>
-      </c>
-      <c r="E12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="1">
-        <v>128</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="1">
-        <v>190</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="1">
-        <v>49</v>
-      </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="1">
-        <v>98</v>
-      </c>
-      <c r="E16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>50</v>
-      </c>
-      <c r="C17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="1">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="1">
-        <v>150</v>
-      </c>
-      <c r="E18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
shopping page Search OK
</commit_message>
<xml_diff>
--- a/designDocument/workman-description.xlsx
+++ b/designDocument/workman-description.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xuant\Desktop\Module1\Module1_workman\designDocument\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72D756F4-1297-4F57-91B4-03E9168A4C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43AA81CA-F551-4224-9415-A3FB55ECC2E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="795" windowWidth="15375" windowHeight="9210" tabRatio="709" activeTab="2" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
+    <workbookView xWindow="13930" yWindow="40" windowWidth="15180" windowHeight="10240" tabRatio="709" firstSheet="2" activeTab="5" xr2:uid="{8F78B35A-A057-42E2-BE4F-2444DF86A27E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -1436,8 +1436,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1198842" y="7340602"/>
-          <a:ext cx="7240120" cy="2890851"/>
+          <a:off x="1206637" y="7311369"/>
+          <a:ext cx="7182954" cy="2876235"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -1786,8 +1786,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1205192" y="1823572"/>
-          <a:ext cx="7233770" cy="2890851"/>
+          <a:off x="1212987" y="1821623"/>
+          <a:ext cx="7176604" cy="2876235"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -3990,8 +3990,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1198842" y="11971806"/>
-          <a:ext cx="7240120" cy="2887676"/>
+          <a:off x="1206637" y="11919187"/>
+          <a:ext cx="7182954" cy="2873060"/>
           <a:chOff x="3175373" y="1595719"/>
           <a:chExt cx="7161119" cy="2834822"/>
         </a:xfrm>
@@ -22104,7 +22104,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.140625" customWidth="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" customWidth="1"/>
@@ -22455,8 +22455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EFD0586-BC3F-4075-B66A-03FF886CAA45}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22470,11 +22470,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D800F0-F99C-47B6-B0F4-3731F0185DB9}">
   <dimension ref="A1:AQ101"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="X13" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="X49" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AA24" sqref="AA24"/>
+      <selection pane="bottomRight" activeCell="Z55" sqref="Z55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22909,8 +22909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A55527AE-C7AB-4C6E-A279-E068211F1548}">
   <dimension ref="A1:S60"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23164,8 +23164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726A8A91-2E1C-4E34-A304-FBDB9334D0CB}">
   <dimension ref="A1:V19"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>